<commit_message>
adding more styles and a second sheet to the example xlsx
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="my_sheet 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">one</t>
   </si>
@@ -92,6 +93,55 @@
   </si>
   <si>
     <t xml:space="preserve">italic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This one has a carriage
+Return</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">this </t>
+    </r>
+    <r>
+      <rPr>
+        <strike val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">one is striked</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> out</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">underlined</t>
   </si>
 </sst>
 </file>
@@ -101,7 +151,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -132,6 +182,20 @@
     </font>
     <font>
       <i val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <strike val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -180,7 +244,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -190,6 +254,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -212,13 +284,13 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -279,4 +351,62 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>